<commit_message>
added search for errors
</commit_message>
<xml_diff>
--- a/devices.xlsx
+++ b/devices.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="31125" yWindow="3075" windowWidth="21600" windowHeight="11385" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="23910" yWindow="3120" windowWidth="27405" windowHeight="11385" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="devices" sheetId="1" state="visible" r:id="rId1"/>
@@ -367,54 +367,455 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="21.140625" customWidth="1" min="1" max="1"/>
     <col width="28.5703125" customWidth="1" min="2" max="2"/>
+    <col width="20.5703125" customWidth="1" min="3" max="3"/>
+    <col width="26.85546875" bestFit="1" customWidth="1" min="4" max="4"/>
+    <col width="22.5703125" customWidth="1" min="5" max="5"/>
+    <col width="14.42578125" bestFit="1" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>devices</t>
+          <t>ComputerName</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>PortName</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>DriverName</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Location</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>MAC</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Vendor</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>www.google.com</t>
+          <t>sykpvps01</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>172.217.9.228</t>
+          <t>tp16n0sc</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>10.1.1.2</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>HP LaserJet 4000 Series PCL 5</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Nursing Admin</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Online</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>0050.7966.6803</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Private</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>www.yahoo.com</t>
+          <t>sykpvps02</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>72.30.35.9</t>
+          <t>tp16n0sc</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>10.1.1.3</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>HP LaserJet 4000 Series PCL 5</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Lobby</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Online</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>0050.7966.6809</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Private</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>sykpvps03</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>tp16n0sc</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>10.1.1.4</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>HP LaserJet 4000 Series PCL 5</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Lab2</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Online</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>0050.7966.6804</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Private</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>sykpvps04</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>tp16n0sc</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>10.1.1.5</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>HP LaserJet 4000 Series PCL 5</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Nursing Admin</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Online</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>0050.7966.680a</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Private</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>sykpvps05</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>tp16n0sc</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>10.1.1.6</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>HP LaserJet 4000 Series PCL 5</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Lobby</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Online</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>0050.7966.6805</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Private</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>sykpvps06</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>tp16n0sc</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>10.1.1.7</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>HP LaserJet 4000 Series PCL 5</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Lab2</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Online</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>0050.7966.680b</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Private</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>sykpvps07</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>tp16n0sc</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>10.1.1.8</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>HP LaserJet 4000 Series PCL 5</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Nursing Admin</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Online</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>0050.7966.6806</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Private</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>sykpvps08</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>tp16n0sc</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>10.1.1.9</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>HP LaserJet 4000 Series PCL 5</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Lobby</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Online</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>0050.7966.680c</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Private</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>sykpvps09</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>tp16n0sc</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>10.1.1.10</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>HP LaserJet 4000 Series PCL 5</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Lab3</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Online</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>0050.7966.6808</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Private</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>10.1.1.11</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Inactive</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A2" r:id="rId1"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A3" r:id="rId2"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>